<commit_message>
Sem van der Hoeven estimated hours filled in
</commit_message>
<xml_diff>
--- a/doc/sprint1/backlog_sprint1edit.xlsx
+++ b/doc/sprint1/backlog_sprint1edit.xlsx
@@ -5,26 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaanS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TU Delft\CSE1105 OOP project\OOP Project SourceTree\doc\sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15115B9D-3082-4D07-B127-14C4048B76F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33A4D63-2B7E-44AC-8392-9C48BAD32F9C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B9BA45A6-7D86-4CB5-8CFC-AD578DCA598C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B9BA45A6-7D86-4CB5-8CFC-AD578DCA598C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -661,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3B02A8-2A8A-4F73-B62F-9E2AE709592E}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -986,7 +980,9 @@
         <f>F18+F20+F25+F24</f>
         <v>6</v>
       </c>
-      <c r="D11" s="21"/>
+      <c r="D11" s="21">
+        <v>5</v>
+      </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>

</xml_diff>

<commit_message>
Ceren Ugurlu estimated hours filled in
</commit_message>
<xml_diff>
--- a/doc/sprint1/backlog_sprint1edit.xlsx
+++ b/doc/sprint1/backlog_sprint1edit.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21421"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TU Delft\CSE1105 OOP project\OOP Project SourceTree\doc\sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33A4D63-2B7E-44AC-8392-9C48BAD32F9C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{766735C9-32F4-40CC-8DB7-7F9498E408AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B9BA45A6-7D86-4CB5-8CFC-AD578DCA598C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -97,9 +103,6 @@
   </si>
   <si>
     <t>&lt;-</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>A</t>
@@ -357,7 +360,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -655,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3B02A8-2A8A-4F73-B62F-9E2AE709592E}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0" xr3:uid="{DA522C76-A1E7-597E-BFF8-8E3344F5E2BF}">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1128,11 +1131,11 @@
       <c r="E15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>24</v>
+      <c r="F15" s="4">
+        <v>2</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="15"/>
@@ -1157,10 +1160,10 @@
     <row r="16" spans="1:26">
       <c r="A16" s="1"/>
       <c r="B16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>7</v>
@@ -1172,7 +1175,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1194,13 +1197,13 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="25.5">
+    <row r="17" spans="1:26">
       <c r="A17" s="1"/>
       <c r="B17" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>8</v>
@@ -1212,7 +1215,7 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1237,10 +1240,10 @@
     <row r="18" spans="1:26" ht="25.5">
       <c r="A18" s="1"/>
       <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>6</v>
@@ -1252,7 +1255,7 @@
         <v>0.5</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1277,10 +1280,10 @@
     <row r="19" spans="1:26">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>8</v>
@@ -1314,13 +1317,13 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="25.5">
+    <row r="20" spans="1:26">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>6</v>
@@ -1332,7 +1335,7 @@
         <v>0.5</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1357,10 +1360,10 @@
     <row r="21" spans="1:26">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>
@@ -1372,7 +1375,7 @@
         <v>0.5</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1397,7 +1400,7 @@
     <row r="22" spans="1:26">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>23</v>
@@ -1412,7 +1415,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1440,13 +1443,13 @@
         <v>18</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="E23" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" s="4">
         <v>4</v>
@@ -1474,13 +1477,13 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26" ht="25.5">
+    <row r="24" spans="1:26">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>6</v>
@@ -1520,13 +1523,13 @@
         <v>18</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="4">
         <v>4</v>
@@ -1554,13 +1557,13 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="25.5">
+    <row r="26" spans="1:26">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>9</v>
@@ -1568,11 +1571,11 @@
       <c r="E26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>24</v>
+      <c r="F26" s="4">
+        <v>0.5</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1597,10 +1600,10 @@
     <row r="27" spans="1:26">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>9</v>
@@ -1608,8 +1611,8 @@
       <c r="E27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>24</v>
+      <c r="F27" s="4">
+        <v>6</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>21</v>
@@ -1637,10 +1640,10 @@
     <row r="28" spans="1:26" ht="25.5">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>9</v>
@@ -1648,8 +1651,8 @@
       <c r="E28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>24</v>
+      <c r="F28" s="4">
+        <v>1.5</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>21</v>

</xml_diff>